<commit_message>
change best model to correct one
</commit_message>
<xml_diff>
--- a/model/metrics/metrics.xlsx
+++ b/model/metrics/metrics.xlsx
@@ -481,29 +481,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1024_3_000033_c</t>
+          <t>1024_3_000033_h</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8662891811794705</v>
+        <v>0.8661446041531033</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8424848901163922</v>
+        <v>0.8445808004347161</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9280086891673268</v>
+        <v>0.9243334039168646</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2075357977059718</v>
+        <v>0.2034571644607057</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8831811735081191</v>
+        <v>0.8826592541663918</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9322116312264431</v>
+        <v>0.9323465529848501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>